<commit_message>
Interface api_service (non aboutie)
</commit_message>
<xml_diff>
--- a/Documentation/Responsabilités.xlsx
+++ b/Documentation/Responsabilités.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\AndroidStudioProjects\quizzy\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D677557-9C03-4940-939C-DACB17E1F700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52C8257-6D53-497B-B20F-938CB6A00EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>Tâche</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Android Studio, Création JSON</t>
+  </si>
+  <si>
+    <t>Mise en fonctionnement de l'API</t>
+  </si>
+  <si>
+    <t>Android Studio, VS Code</t>
   </si>
 </sst>
 </file>
@@ -648,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B237FC8F-6C56-5C4D-A049-31CB1F31A8AE}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,7 +771,7 @@
       </c>
       <c r="G5" s="12">
         <f>SUMIF(B:B,"Pierre",C:C)</f>
-        <v>9.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -787,7 +793,7 @@
       </c>
       <c r="G6" s="14">
         <f>SUM(C:C)</f>
-        <v>28.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -801,31 +807,33 @@
         <v>4</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -837,13 +845,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>17</v>
@@ -852,27 +860,25 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -886,10 +892,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -897,14 +903,16 @@
       <c r="D13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -916,13 +924,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>17</v>
@@ -934,10 +942,10 @@
         <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>17</v>
@@ -949,7 +957,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -961,13 +969,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>17</v>
@@ -976,41 +984,49 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4">
         <v>1.5</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="9"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1048,6 +1064,13 @@
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>